<commit_message>
add pie and scatter
</commit_message>
<xml_diff>
--- a/dist/xlsx/templates/template.xlsx
+++ b/dist/xlsx/templates/template.xlsx
@@ -6,6 +6,8 @@
     <sheet state="visible" name="SheetTemplate" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="barTemplate" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="lineTemplate" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="pieTemplate" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="scatterTemplate" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +15,35 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>tot</t>
+  </si>
+  <si>
+    <t>frot</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>bbb</t>
+  </si>
+  <si>
+    <t>ccc</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -168,11 +198,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1229208011"/>
-        <c:axId val="1283735709"/>
+        <c:axId val="1287661931"/>
+        <c:axId val="1679951776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1229208011"/>
+        <c:axId val="1287661931"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -224,10 +254,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1283735709"/>
+        <c:crossAx val="1679951776"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1283735709"/>
+        <c:axId val="1679951776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -302,7 +332,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1229208011"/>
+        <c:crossAx val="1287661931"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -338,7 +368,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr lvl="0">
-              <a:defRPr b="0">
+              <a:defRPr b="0" sz="2400">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -346,13 +376,13 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0">
+              <a:rPr b="0" sz="2400">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>line</a:t>
+              <a:t>tot and frot</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -365,8 +395,13 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>lineTemplate!$A$2</c:f>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln cmpd="sng">
+            <a:ln cmpd="sng" w="19050">
               <a:solidFill>
                 <a:srgbClr val="4285F4"/>
               </a:solidFill>
@@ -388,12 +423,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>lineTemplate!$A$1:$B$1</c:f>
+              <c:f>lineTemplate!$B$1:$D$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>lineTemplate!$A$2:$B$2</c:f>
+              <c:f>lineTemplate!$B$2:$D$2</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -402,8 +437,13 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>lineTemplate!$A$3</c:f>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln cmpd="sng">
+            <a:ln cmpd="sng" w="19050">
               <a:solidFill>
                 <a:srgbClr val="EA4335"/>
               </a:solidFill>
@@ -425,22 +465,22 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>lineTemplate!$A$1:$B$1</c:f>
+              <c:f>lineTemplate!$B$1:$D$1</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>lineTemplate!$A$3:$B$3</c:f>
+              <c:f>lineTemplate!$B$3:$D$3</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="943746936"/>
-        <c:axId val="1716265905"/>
+        <c:axId val="1156191164"/>
+        <c:axId val="657065325"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="943746936"/>
+        <c:axId val="1156191164"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -467,7 +507,7 @@
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                   </a:rPr>
-                  <a:t/>
+                  <a:t>dd</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -492,10 +532,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1716265905"/>
+        <c:crossAx val="657065325"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1716265905"/>
+        <c:axId val="657065325"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -570,7 +610,417 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="943746936"/>
+        <c:crossAx val="1156191164"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>bbb and ccc</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>pieTemplate!$A$2</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>pieTemplate!$B$1:$D$1</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>pieTemplate!$B$2:$D$2</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>aaa and bbb</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>scatterTemplate!$A$2</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>scatterTemplate!$B$1:$D$1</c:f>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>scatterTemplate!$B$2:$D$2</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>scatterTemplate!$A$3</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>scatterTemplate!$B$1:$D$1</c:f>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>scatterTemplate!$B$3:$D$3</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="195423032"/>
+        <c:axId val="258715511"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="195423032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="258715511"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="258715511"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="195423032"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -636,13 +1086,73 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 2" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3533775"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 3" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3533775"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 4" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -926,27 +1436,153 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
         <v>0.0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="C1" s="1">
         <v>1.0</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2.0</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
         <v>2.0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2" s="1">
         <v>3.0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
         <v>4.0</v>
       </c>
+      <c r="C3" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B3" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="C3" s="1">
         <v>5.0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>6.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>